<commit_message>
added Total Giftcard Spend line
</commit_message>
<xml_diff>
--- a/Ecom Modelling ASOS.xlsx
+++ b/Ecom Modelling ASOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexmclaughlin/Library/CloudStorage/OneDrive-SubtvU/Alex-McLaughlin/Loyality Scheme/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52459A93-EEBA-E046-AEF6-96C38F28B4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90E3E6D-4A8C-7C48-A226-A4F07F129BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21340" xr2:uid="{A0095DDC-8E5F-8542-BAAD-5C4BF5024CD1}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{A0095DDC-8E5F-8542-BAAD-5C4BF5024CD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
   <si>
     <t>Conversion to Customers</t>
   </si>
@@ -65,21 +65,9 @@
     <t>App Users From Rockbox</t>
   </si>
   <si>
-    <t>Average Yearly Purchases</t>
-  </si>
-  <si>
     <t>Percentage Spend on Fashion</t>
   </si>
   <si>
-    <t>UCAS?</t>
-  </si>
-  <si>
-    <t>ASOS Market Share</t>
-  </si>
-  <si>
-    <t>Proportion Spend on Giftcards</t>
-  </si>
-  <si>
     <t>Academic Weeks</t>
   </si>
   <si>
@@ -89,12 +77,6 @@
     <t>Average Yearly Spend Fashion</t>
   </si>
   <si>
-    <t>Average Yearly Spend Fashion Subtv</t>
-  </si>
-  <si>
-    <t>Average Yearly Spend ASOS Subtv</t>
-  </si>
-  <si>
     <t>Total Spend ASOS Subtv</t>
   </si>
   <si>
@@ -246,6 +228,9 @@
   </si>
   <si>
     <t>Superdry</t>
+  </si>
+  <si>
+    <t>Column2</t>
   </si>
 </sst>
 </file>
@@ -340,7 +325,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -399,12 +384,24 @@
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -564,15 +561,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1066800</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>1513840</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>40640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -595,8 +592,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1066800" y="4749800"/>
-          <a:ext cx="1930400" cy="1549400"/>
+          <a:off x="1513840" y="1869440"/>
+          <a:ext cx="1935480" cy="1549400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -669,33 +666,34 @@
   <autoFilter ref="E1:H23" xr:uid="{F48752E7-4379-4E4B-AF12-DDED6F5DA79C}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{518D7F3D-62A8-8741-A135-79C976D1848C}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{15885B75-A5DE-0541-B966-6FD06E9FF2AE}" name="Pessimistic" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{753D3EEE-4AE2-7140-AA84-7D4D0E47B005}" name="Likely" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{7FB7FDD2-BC57-584C-9A24-1132D54E8284}" name="Optimistic" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{15885B75-A5DE-0541-B966-6FD06E9FF2AE}" name="Pessimistic" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{753D3EEE-4AE2-7140-AA84-7D4D0E47B005}" name="Likely" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{7FB7FDD2-BC57-584C-9A24-1132D54E8284}" name="Optimistic" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DDA67F96-0A11-E14E-A21A-F583E73D3EA7}" name="Table2" displayName="Table2" ref="L1:O22" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="L1:O22" xr:uid="{DDA67F96-0A11-E14E-A21A-F583E73D3EA7}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{70240E8F-9647-9443-BC52-5922B0C73132}" name="Column1" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{0E467C07-020D-FF4D-BC44-14F5D0B67063}" name="Pessimistic" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{63B56CA1-7EDC-CC43-878E-925429763187}" name="Likely" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{91FE7774-526B-4240-8DD8-32ACEDFEF41D}" name="Optimistic" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DDA67F96-0A11-E14E-A21A-F583E73D3EA7}" name="Table2" displayName="Table2" ref="L1:P22" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="L1:P22" xr:uid="{DDA67F96-0A11-E14E-A21A-F583E73D3EA7}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{70240E8F-9647-9443-BC52-5922B0C73132}" name="Column1" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{0E467C07-020D-FF4D-BC44-14F5D0B67063}" name="Pessimistic" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{63B56CA1-7EDC-CC43-878E-925429763187}" name="Likely" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{91FE7774-526B-4240-8DD8-32ACEDFEF41D}" name="Optimistic" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{EA300B35-0C13-1946-AD1C-30E08E6B8E9E}" name="Column2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2675A0D7-3747-704C-A448-6C6F196AE969}" name="Table24" displayName="Table24" ref="I27:J35" totalsRowShown="0" dataDxfId="3" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2675A0D7-3747-704C-A448-6C6F196AE969}" name="Table24" displayName="Table24" ref="I27:J35" totalsRowShown="0" dataDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="I27:J35" xr:uid="{2675A0D7-3747-704C-A448-6C6F196AE969}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{ECF93E29-F768-5545-8600-B1AD534626BA}" name="Brand" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{2A4BC554-D55F-CC4A-A1A1-80355DCDB266}" name="Discount" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{ECF93E29-F768-5545-8600-B1AD534626BA}" name="Brand" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{2A4BC554-D55F-CC4A-A1A1-80355DCDB266}" name="Discount" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1020,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E321E73A-F259-E94B-B600-4AEF6EA281B8}">
   <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection sqref="A1:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1038,43 +1036,41 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="E1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="I1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="L1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="M1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="N1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="O1" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+      <c r="P1" s="29" t="s">
+        <v>64</v>
       </c>
       <c r="S1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>718826</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="E2" t="s">
         <v>5</v>
       </c>
@@ -1103,23 +1099,19 @@
         <f>1.05*N2</f>
         <v>754767.3</v>
       </c>
+      <c r="P2" s="28"/>
       <c r="S2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="T2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0.04</v>
-      </c>
+      <c r="B3" s="4"/>
       <c r="E3" t="s">
         <v>2</v>
       </c>
@@ -1144,24 +1136,19 @@
       <c r="O3" s="12">
         <v>4.4999999999999998E-2</v>
       </c>
+      <c r="P3" s="28"/>
       <c r="S3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="T3" s="2">
         <v>0.1</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1">
-        <f>B2*B3</f>
-        <v>28753.040000000001</v>
-      </c>
+      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" t="s">
@@ -1194,26 +1181,20 @@
         <f>O2*O3</f>
         <v>33964.5285</v>
       </c>
+      <c r="P4" s="28"/>
       <c r="S4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="T4" s="2">
         <v>0.1</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>4300000</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="3"/>
       <c r="E5" t="s">
         <v>3</v>
       </c>
@@ -1241,14 +1222,10 @@
       <c r="O5" s="10">
         <v>2000000</v>
       </c>
+      <c r="P5" s="28"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1E-3</v>
-      </c>
+      <c r="B6" s="4"/>
       <c r="E6" t="s">
         <v>4</v>
       </c>
@@ -1265,23 +1242,18 @@
         <v>4</v>
       </c>
       <c r="M6" s="12">
-        <v>5.0000000000000001E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="N6" s="12">
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="O6" s="12">
-        <v>2E-3</v>
-      </c>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="P6" s="28"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1">
-        <f>B5*B6</f>
-        <v>4300</v>
-      </c>
+      <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" t="s">
@@ -1304,25 +1276,20 @@
       </c>
       <c r="M7" s="10">
         <f>M5*M6</f>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="N7" s="10">
         <f>N5*N6</f>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="O7" s="10">
         <f>O5*O6</f>
-        <v>4000</v>
-      </c>
+        <v>6000</v>
+      </c>
+      <c r="P7" s="28"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1">
-        <f>B4+B7</f>
-        <v>33053.040000000001</v>
-      </c>
+      <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" t="s">
@@ -1345,24 +1312,19 @@
       </c>
       <c r="M8" s="10">
         <f>M4+M7</f>
-        <v>18072.1175</v>
+        <v>19072.1175</v>
       </c>
       <c r="N8" s="10">
         <f>N4+N7</f>
-        <v>27158.910000000003</v>
+        <v>29158.910000000003</v>
       </c>
       <c r="O8" s="10">
         <f>O4+O7</f>
-        <v>37964.5285</v>
-      </c>
+        <v>39964.5285</v>
+      </c>
+      <c r="P8" s="28"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
       <c r="E9" t="s">
         <v>0</v>
       </c>
@@ -1376,10 +1338,10 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="I9" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="L9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="M9" s="19">
         <f>176840/17755</f>
@@ -1393,16 +1355,12 @@
         <f>M9*1.1</f>
         <v>10.956012390875809</v>
       </c>
+      <c r="P9" s="28"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="5">
-        <v>30</v>
-      </c>
+      <c r="B10" s="5"/>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F10" s="11">
         <v>15</v>
@@ -1414,33 +1372,26 @@
         <v>25</v>
       </c>
       <c r="L10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="M10" s="10">
         <f>M9*M8</f>
-        <v>179998.49387214868</v>
+        <v>189958.50513658125</v>
       </c>
       <c r="N10" s="10">
         <f>N9*N8</f>
-        <v>284028.2020061955</v>
+        <v>304944.22566150385</v>
       </c>
       <c r="O10" s="10">
         <f>O9*O8</f>
-        <v>415939.8446597578</v>
-      </c>
+        <v>437851.86944150942</v>
+      </c>
+      <c r="P10" s="28"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4">
-        <v>0.17</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B11" s="4"/>
+      <c r="E11" t="s">
         <v>11</v>
-      </c>
-      <c r="E11" t="s">
-        <v>15</v>
       </c>
       <c r="F11" s="13">
         <v>25</v>
@@ -1452,7 +1403,7 @@
         <v>35</v>
       </c>
       <c r="L11" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="M11" s="12">
         <f>148254/176840</f>
@@ -1466,16 +1417,12 @@
         <f>148254/176840</f>
         <v>0.83835105179823566</v>
       </c>
+      <c r="P11" s="28"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="4">
-        <v>0.5</v>
-      </c>
+      <c r="B12" s="4"/>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" s="15">
         <v>0.17</v>
@@ -1487,33 +1434,28 @@
         <v>0.17</v>
       </c>
       <c r="L12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="M12" s="10">
         <f>M11*M10</f>
-        <v>150901.92665981411</v>
+        <v>159251.91257927346</v>
       </c>
       <c r="N12" s="10">
         <f t="shared" ref="N12:O12" si="3">N11*N10</f>
-        <v>238115.34189225573</v>
+        <v>255650.31232312028</v>
       </c>
       <c r="O12" s="10">
         <f t="shared" si="3"/>
-        <v>348703.60625530273</v>
-      </c>
+        <v>367073.57527811319</v>
+      </c>
+      <c r="P12" s="28"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="5">
-        <f>B9*B10*B11*B12</f>
-        <v>12.750000000000002</v>
-      </c>
+      <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F13" s="11">
         <f>F10*F12</f>
@@ -1529,7 +1471,7 @@
       </c>
       <c r="J13" s="9"/>
       <c r="L13" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="M13" s="19">
         <f>2631874/148254</f>
@@ -1543,19 +1485,14 @@
         <f>Table2[[#This Row],[Likely]]+1</f>
         <v>19.75246536349778</v>
       </c>
+      <c r="P13" s="28"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="4">
-        <f>B21/B20</f>
-        <v>0.16066066066066065</v>
-      </c>
+      <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F14" s="14">
         <f>F10*F11*F12</f>
@@ -1571,33 +1508,28 @@
       </c>
       <c r="J14" s="9"/>
       <c r="L14" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="M14" s="10">
         <f>M13*M12</f>
-        <v>2678881.2263134322</v>
+        <v>2827114.0621343283</v>
       </c>
       <c r="N14" s="10">
         <f t="shared" ref="N14:O14" si="6">N13*N12</f>
-        <v>4465249.7013519574</v>
+        <v>4794073.6270067031</v>
       </c>
       <c r="O14" s="10">
         <f t="shared" si="6"/>
-        <v>6887755.9046846349</v>
-      </c>
+        <v>7250608.081536226</v>
+      </c>
+      <c r="P14" s="28"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="5">
-        <f>B13*B14</f>
-        <v>2.0484234234234235</v>
-      </c>
+      <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F15" s="14">
         <v>37</v>
@@ -1609,10 +1541,10 @@
         <v>37</v>
       </c>
       <c r="I15" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="L15" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="M15" s="12">
         <v>0.02</v>
@@ -1623,22 +1555,17 @@
       <c r="O15" s="12">
         <v>0.06</v>
       </c>
-      <c r="P15" t="s">
-        <v>43</v>
+      <c r="P15" s="28" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="7">
-        <f>B15*B8</f>
-        <v>67706.62135135135</v>
-      </c>
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F16" s="11">
         <v>32</v>
@@ -1650,33 +1577,29 @@
         <v>32</v>
       </c>
       <c r="L16" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="M16" s="10">
         <f>M14*M15</f>
-        <v>53577.624526268643</v>
+        <v>56542.281242686564</v>
       </c>
       <c r="N16" s="10">
         <f t="shared" ref="N16:O16" si="7">N14*N15</f>
-        <v>178609.98805407831</v>
+        <v>191762.94508026814</v>
       </c>
       <c r="O16" s="10">
         <f t="shared" si="7"/>
-        <v>413265.35428107809</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="8">
-        <f>B16/B10</f>
-        <v>2256.8873783783783</v>
-      </c>
+        <v>435036.48489217355</v>
+      </c>
+      <c r="P16" s="28"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F17" s="14">
         <f t="shared" ref="F17" si="8">F15*F16</f>
@@ -1691,7 +1614,7 @@
         <v>1184</v>
       </c>
       <c r="L17" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M17" s="12">
         <v>1.4999999999999999E-2</v>
@@ -1702,18 +1625,14 @@
       <c r="O17" s="12">
         <v>2.5000000000000001E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="5">
-        <v>37</v>
-      </c>
+      <c r="P17" s="28"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F18" s="14">
         <v>214</v>
@@ -1725,33 +1644,28 @@
         <v>214</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="L18" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="M18" s="20">
         <f>M16*M17</f>
-        <v>803.66436789402962</v>
+        <v>848.1342186402984</v>
       </c>
       <c r="N18" s="20">
         <f t="shared" ref="N18:O18" si="11">N16*N17</f>
-        <v>3572.1997610815661</v>
+        <v>3835.258901605363</v>
       </c>
       <c r="O18" s="20">
         <f t="shared" si="11"/>
-        <v>10331.633857026953</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19">
-        <v>36</v>
-      </c>
+        <v>10875.91212230434</v>
+      </c>
+      <c r="P18" s="28"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F19" s="15">
         <f>F18/F17</f>
@@ -1766,7 +1680,7 @@
         <v>0.18074324324324326</v>
       </c>
       <c r="L19" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="M19" s="21">
         <v>0.2</v>
@@ -1777,19 +1691,14 @@
       <c r="O19" s="21">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="5">
-        <f>B18*B19</f>
-        <v>1332</v>
-      </c>
+      <c r="P19" s="28"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F20" s="15">
         <f>F19*1.3</f>
@@ -1804,10 +1713,10 @@
         <v>0.23496621621621624</v>
       </c>
       <c r="I20" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="L20" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="M20" s="13">
         <v>25</v>
@@ -1818,19 +1727,13 @@
       <c r="O20" s="13">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="5">
-        <v>214</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="P20" s="28"/>
+    </row>
+    <row r="21" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="3"/>
       <c r="E21" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F21" s="14">
         <f>F14*F20</f>
@@ -1847,24 +1750,25 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="22" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="M21" s="23">
         <f>M16*M17*M20*M19</f>
-        <v>4018.321839470148</v>
+        <v>4240.6710932014921</v>
       </c>
       <c r="N21" s="23">
         <f>N16*N17*N20*N19</f>
-        <v>26791.498208111745</v>
+        <v>28764.441762040224</v>
       </c>
       <c r="O21" s="23">
         <f>O16*O17*O20*O19</f>
-        <v>108482.155498783</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+        <v>114197.07728419556</v>
+      </c>
+      <c r="P21" s="28"/>
+    </row>
+    <row r="22" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="E22" s="16" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F22" s="17">
         <f>F21*F8*F9</f>
@@ -1880,24 +1784,25 @@
       </c>
       <c r="J22" s="3"/>
       <c r="L22" s="22" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="M22" s="24">
         <f>M21/M20</f>
-        <v>160.73287357880591</v>
+        <v>169.6268437280597</v>
       </c>
       <c r="N22" s="24">
         <f t="shared" ref="N22:O22" si="14">N21/N20</f>
-        <v>893.04994027039152</v>
+        <v>958.81472540134075</v>
       </c>
       <c r="O22" s="24">
         <f t="shared" si="14"/>
-        <v>3099.4901571080859</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+        <v>3262.7736366913018</v>
+      </c>
+      <c r="P22" s="28"/>
+    </row>
+    <row r="23" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="E23" s="16" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F23" s="18">
         <f>F22/F11</f>
@@ -1912,60 +1817,60 @@
         <v>2843.3716388497683</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J26" s="9"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I27" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="J27" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I28" s="25" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="J28" s="26">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I29" s="25" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="J29" s="26">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I30" s="25" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="J30" s="26">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I31" s="25" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="J31" s="26">
         <v>8.5</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="I32" s="25" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="J32" s="26">
         <v>10</v>
@@ -1973,7 +1878,7 @@
     </row>
     <row r="33" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I33" s="25" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J33" s="26">
         <v>8</v>
@@ -1981,7 +1886,7 @@
     </row>
     <row r="34" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I34" s="25" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="J34" s="26">
         <v>8.5</v>
@@ -1989,7 +1894,7 @@
     </row>
     <row r="35" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I35" s="25" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="J35" s="26">
         <v>7</v>
@@ -2003,21 +1908,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C21" r:id="rId1" xr:uid="{EE712FBB-E5DF-034D-8CBD-E2A9292D95A2}"/>
-    <hyperlink ref="C5" r:id="rId2" xr:uid="{096D907E-F50E-E14B-8914-5B4294B9E5FF}"/>
-    <hyperlink ref="U2" r:id="rId3" xr:uid="{3F70E09F-A2D8-7B4B-8C6F-51BF62512ECC}"/>
-    <hyperlink ref="U3" r:id="rId4" xr:uid="{FE13424D-DBBF-E746-9514-413D2865DFC3}"/>
-    <hyperlink ref="U4" r:id="rId5" xr:uid="{F93776DA-60D8-E04E-AD93-DD3F6AA39F81}"/>
-    <hyperlink ref="I18" r:id="rId6" xr:uid="{8CEA7267-693A-B04F-AB94-8CE6C4CE61E7}"/>
-    <hyperlink ref="I5" r:id="rId7" xr:uid="{714DC32F-8B46-8B48-AB3B-4F98EE39C0E1}"/>
+    <hyperlink ref="U2" r:id="rId1" xr:uid="{3F70E09F-A2D8-7B4B-8C6F-51BF62512ECC}"/>
+    <hyperlink ref="U3" r:id="rId2" xr:uid="{FE13424D-DBBF-E746-9514-413D2865DFC3}"/>
+    <hyperlink ref="U4" r:id="rId3" xr:uid="{F93776DA-60D8-E04E-AD93-DD3F6AA39F81}"/>
+    <hyperlink ref="I18" r:id="rId4" xr:uid="{8CEA7267-693A-B04F-AB94-8CE6C4CE61E7}"/>
+    <hyperlink ref="I5" r:id="rId5" xr:uid="{714DC32F-8B46-8B48-AB3B-4F98EE39C0E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId8"/>
+  <drawing r:id="rId6"/>
   <tableParts count="3">
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
-    <tablePart r:id="rId10"/>
-    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>